<commit_message>
a lot of analysis and data
</commit_message>
<xml_diff>
--- a/online_experiment/analysis/short_answers/scored/b2_b3/tony/32.xlsx
+++ b/online_experiment/analysis/short_answers/scored/b2_b3/tony/32.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -54,15 +54,6 @@
   </si>
   <si>
     <t>2020-07-30</t>
-  </si>
-  <si>
-    <t>5ed773ad2006c61f224dc9a0</t>
-  </si>
-  <si>
-    <t>"  "</t>
-  </si>
-  <si>
-    <t>" "</t>
   </si>
   <si>
     <t>5c730ca1f674750001df8d09</t>
@@ -174,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -182,6 +173,11 @@
     </font>
     <font>
       <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
@@ -212,7 +208,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -223,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -242,36 +238,6 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
         <color indexed="10"/>
       </bottom>
       <diagonal/>
@@ -281,22 +247,7 @@
         <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
@@ -308,7 +259,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="10"/>
@@ -323,16 +274,88 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top style="thin">
         <color indexed="10"/>
-      </left>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="15"/>
       </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
       </bottom>
       <diagonal/>
     </border>
@@ -342,48 +365,60 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,10 +439,11 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="fffeffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -424,10 +460,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -621,14 +657,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -643,35 +680,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -924,14 +955,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1220,7 +1257,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1501,11 +1538,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U6"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1612,7 +1647,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s" s="8">
         <v>15</v>
@@ -1620,298 +1655,335 @@
       <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="6"/>
+      <c r="H2" t="s" s="8">
+        <v>16</v>
+      </c>
       <c r="I2" s="6">
-        <v>0</v>
-      </c>
-      <c r="J2" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="J2" t="s" s="8">
+        <v>17</v>
+      </c>
       <c r="K2" s="6">
         <v>0</v>
       </c>
-      <c r="L2" s="6"/>
+      <c r="L2" t="s" s="8">
+        <v>18</v>
+      </c>
       <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6"/>
+        <v>2</v>
+      </c>
+      <c r="N2" t="s" s="8">
+        <v>19</v>
+      </c>
       <c r="O2" s="6">
         <v>0</v>
       </c>
-      <c r="P2" s="6"/>
+      <c r="P2" t="s" s="8">
+        <v>20</v>
+      </c>
       <c r="Q2" s="6">
         <v>0</v>
       </c>
       <c r="R2" t="s" s="8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="S2" s="6">
         <v>0</v>
       </c>
       <c r="T2" t="s" s="8">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="U2" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="9">
+      <c r="A3" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="B3" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C3" s="11">
+      <c r="B3" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6">
         <v>32</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="7">
         <v>2</v>
       </c>
-      <c r="E3" s="12">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="I3" s="11">
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6">
         <v>3</v>
       </c>
-      <c r="J3" t="s" s="13">
-        <v>20</v>
-      </c>
-      <c r="K3" s="11">
-        <v>0</v>
-      </c>
-      <c r="L3" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="M3" s="11">
-        <v>2</v>
-      </c>
-      <c r="N3" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="O3" s="11">
-        <v>0</v>
-      </c>
-      <c r="P3" t="s" s="13">
-        <v>23</v>
-      </c>
-      <c r="Q3" s="11">
-        <v>0</v>
-      </c>
-      <c r="R3" t="s" s="13">
-        <v>24</v>
-      </c>
-      <c r="S3" s="11">
-        <v>0</v>
-      </c>
-      <c r="T3" t="s" s="13">
+      <c r="H3" t="s" s="8">
         <v>25</v>
       </c>
-      <c r="U3" s="11">
-        <v>0</v>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s" s="8">
+        <v>26</v>
+      </c>
+      <c r="K3" s="6">
+        <v>3</v>
+      </c>
+      <c r="L3" t="s" s="8">
+        <v>27</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s" s="8">
+        <v>28</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>3</v>
+      </c>
+      <c r="R3" t="s" s="8">
+        <v>30</v>
+      </c>
+      <c r="S3" s="6">
+        <v>3</v>
+      </c>
+      <c r="T3" t="s" s="8">
+        <v>31</v>
+      </c>
+      <c r="U3" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" t="s" s="9">
+      <c r="A4" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>26</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="B4" t="s" s="5">
         <v>32</v>
       </c>
-      <c r="D4" s="12">
+      <c r="C4" s="6">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7">
         <v>2</v>
       </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s" s="13">
-        <v>27</v>
-      </c>
-      <c r="G4" s="11">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s" s="13">
-        <v>28</v>
-      </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s" s="13">
-        <v>29</v>
-      </c>
-      <c r="K4" s="11">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s" s="13">
-        <v>30</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0</v>
-      </c>
-      <c r="N4" t="s" s="13">
-        <v>31</v>
-      </c>
-      <c r="O4" s="11">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s" s="13">
-        <v>32</v>
-      </c>
-      <c r="Q4" s="11">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s" s="13">
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="S4" s="11">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s" s="13">
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s" s="8">
         <v>34</v>
       </c>
-      <c r="U4" s="11">
-        <v>3</v>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" t="s" s="8">
+        <v>39</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" t="s" s="9">
+      <c r="A5" t="s" s="4">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="10">
-        <v>35</v>
-      </c>
-      <c r="C5" s="11">
+      <c r="B5" t="s" s="5">
+        <v>40</v>
+      </c>
+      <c r="C5" s="6">
         <v>32</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="7">
         <v>2</v>
       </c>
-      <c r="E5" s="12">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s" s="13">
-        <v>36</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="I5" s="11">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s" s="13">
-        <v>38</v>
-      </c>
-      <c r="K5" s="11">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s" s="13">
-        <v>37</v>
-      </c>
-      <c r="M5" s="11">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s" s="13">
-        <v>39</v>
-      </c>
-      <c r="O5" s="11">
-        <v>0</v>
-      </c>
-      <c r="P5" t="s" s="13">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="11">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s" s="13">
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s" s="8">
         <v>41</v>
       </c>
-      <c r="S5" s="11">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s" s="13">
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s" s="8">
         <v>42</v>
       </c>
-      <c r="U5" s="11">
-        <v>0</v>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s" s="8">
+        <v>43</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s" s="8">
+        <v>44</v>
+      </c>
+      <c r="M5" s="6">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s" s="8">
+        <v>45</v>
+      </c>
+      <c r="O5" s="6">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s" s="8">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>3</v>
+      </c>
+      <c r="R5" t="s" s="8">
+        <v>46</v>
+      </c>
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" t="s" s="8">
+        <v>47</v>
+      </c>
+      <c r="U5" s="6">
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" t="s" s="9">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s" s="10">
-        <v>43</v>
-      </c>
-      <c r="C6" s="11">
-        <v>32</v>
-      </c>
-      <c r="D6" s="12">
-        <v>2</v>
-      </c>
-      <c r="E6" s="12">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s" s="13">
-        <v>44</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s" s="13">
-        <v>45</v>
-      </c>
-      <c r="I6" s="11">
-        <v>3</v>
-      </c>
-      <c r="J6" t="s" s="13">
-        <v>46</v>
-      </c>
-      <c r="K6" s="11">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s" s="13">
-        <v>47</v>
-      </c>
-      <c r="M6" s="11">
-        <v>3</v>
-      </c>
-      <c r="N6" t="s" s="13">
-        <v>48</v>
-      </c>
-      <c r="O6" s="11">
-        <v>2</v>
-      </c>
-      <c r="P6" t="s" s="13">
-        <v>32</v>
-      </c>
-      <c r="Q6" s="11">
-        <v>3</v>
-      </c>
-      <c r="R6" t="s" s="13">
-        <v>49</v>
-      </c>
-      <c r="S6" s="11">
-        <v>0</v>
-      </c>
-      <c r="T6" t="s" s="13">
-        <v>50</v>
-      </c>
-      <c r="U6" s="11">
-        <v>3</v>
-      </c>
+      <c r="A6" s="9"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="11"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="12"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+      <c r="S7" s="13"/>
+      <c r="T7" s="13"/>
+      <c r="U7" s="14"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="14"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>